<commit_message>
percentage of sales added - still gpt-4
</commit_message>
<xml_diff>
--- a/uploaded_files/cleaned_PL 8 Months.xlsx
+++ b/uploaded_files/cleaned_PL 8 Months.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,47 +481,87 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>Account type</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Account hierarchy</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Difference Jul 2023</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Difference Aug 2023</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Difference Sep 2023</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Difference Oct 2023</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Difference Nov 2023</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Difference Dec 2023</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Difference Jan 2024</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Account type</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Account hierarchy</t>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>% of Sales Jul 2023</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>% of Sales Aug 2023</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>% of Sales Sep 2023</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>% of Sales Oct 2023</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>% of Sales Nov 2023</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>% of Sales Dec 2023</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>% of Sales Jan 2024</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>% of Sales Feb 2024</t>
         </is>
       </c>
     </row>
@@ -539,23 +579,31 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Account group</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Account group</t>
-        </is>
-      </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -571,23 +619,31 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Account group</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Account group</t>
-        </is>
-      </c>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -619,33 +675,57 @@
       <c r="I4" t="n">
         <v>2559356</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
         <v>-106175</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>643511</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>-1250432</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>-1432986</v>
       </c>
-      <c r="N4" t="n">
+      <c r="P4" t="n">
         <v>-1013898</v>
       </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
         <v>2233724</v>
       </c>
-      <c r="P4" t="n">
+      <c r="R4" t="n">
         <v>270299</v>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="n">
+        <v>0.06644788843256125</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.06873486121047148</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.08772274674352348</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.06924023758087035</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.08239442685103626</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.08821322119820894</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.08020275347230982</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.07157972575829276</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -677,33 +757,57 @@
       <c r="I5" t="n">
         <v>4113591</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="n">
         <v>1108239</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>463708</v>
       </c>
-      <c r="L5" t="n">
+      <c r="N5" t="n">
         <v>-1637916</v>
       </c>
-      <c r="M5" t="n">
+      <c r="O5" t="n">
         <v>-1852934</v>
       </c>
-      <c r="N5" t="n">
+      <c r="P5" t="n">
         <v>522635</v>
       </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
         <v>1513555</v>
       </c>
-      <c r="P5" t="n">
+      <c r="R5" t="n">
         <v>-993027</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="n">
+        <v>0.1130337685420959</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.07284060465161003</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.1069772585093241</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.08742890077161664</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.1049240113095453</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.08073473552065188</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.08844817661042247</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.1150483620339575</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -735,33 +839,57 @@
       <c r="I6" t="n">
         <v>673301</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
         <v>297748</v>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>7269</v>
       </c>
-      <c r="L6" t="n">
+      <c r="N6" t="n">
         <v>-471313</v>
       </c>
-      <c r="M6" t="n">
+      <c r="O6" t="n">
         <v>223205</v>
       </c>
-      <c r="N6" t="n">
+      <c r="P6" t="n">
         <v>-517956</v>
       </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
         <v>654854</v>
       </c>
-      <c r="P6" t="n">
+      <c r="R6" t="n">
         <v>-291917</v>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="n">
+        <v>0.02007998711537273</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.009489576446956837</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.01734942340044691</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.01962195075592608</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.01054543738745997</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.01805314038470943</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.0108098149528064</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.01883079217302488</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -793,33 +921,57 @@
       <c r="I7" t="n">
         <v>483172</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
         <v>-24977</v>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>-86589</v>
       </c>
-      <c r="L7" t="n">
+      <c r="N7" t="n">
         <v>-222482</v>
       </c>
-      <c r="M7" t="n">
+      <c r="O7" t="n">
         <v>-553532</v>
       </c>
-      <c r="N7" t="n">
+      <c r="P7" t="n">
         <v>-318654</v>
       </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
         <v>252799</v>
       </c>
-      <c r="P7" t="n">
+      <c r="R7" t="n">
         <v>470998</v>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="n">
+        <v>2.565893856092838e-05</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.0008794454702557073</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.007211491843380892</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.008859353623086043</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.01807446566317468</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.02102758323569716</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.02704466137415121</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.01351328977058519</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -851,36 +1003,60 @@
       <c r="I8" t="n">
         <v>7829420</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Subtotals</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
         <v>1274835</v>
       </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
         <v>1027899</v>
       </c>
-      <c r="L8" t="n">
+      <c r="N8" t="n">
         <v>-3582143</v>
       </c>
-      <c r="M8" t="n">
+      <c r="O8" t="n">
         <v>-3616247</v>
       </c>
-      <c r="N8" t="n">
+      <c r="P8" t="n">
         <v>-1327873</v>
       </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
         <v>4654932</v>
       </c>
-      <c r="P8" t="n">
+      <c r="R8" t="n">
         <v>-543647</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Subtotals</t>
-        </is>
+      <c r="S8" t="n">
+        <v>0.1995873030285908</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.1519444877792941</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.2192609204966754</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.1851504427314991</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.2159383412112162</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.2080286803392674</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.2065054064096899</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.2189721697358603</v>
       </c>
     </row>
     <row r="9">
@@ -897,23 +1073,31 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Account group</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Account group</t>
-        </is>
-      </c>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -945,33 +1129,57 @@
       <c r="I10" t="n">
         <v>770802</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
         <v>240265</v>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
         <v>48583</v>
       </c>
-      <c r="L10" t="n">
+      <c r="N10" t="n">
         <v>-385300</v>
       </c>
-      <c r="M10" t="n">
+      <c r="O10" t="n">
         <v>-269266</v>
       </c>
-      <c r="N10" t="n">
+      <c r="P10" t="n">
         <v>14978</v>
       </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
         <v>346250</v>
       </c>
-      <c r="P10" t="n">
+      <c r="R10" t="n">
         <v>-22083</v>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="n">
+        <v>0.02598112406294036</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.01723743220954991</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.02924262800091392</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.02224691893916238</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.0225839920967717</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.01907634064172989</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.02122142995419382</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.02155768707985273</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1003,33 +1211,57 @@
       <c r="I11" t="n">
         <v>430281</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="n">
         <v>-47296</v>
       </c>
-      <c r="K11" t="n">
+      <c r="M11" t="n">
         <v>4984</v>
       </c>
-      <c r="L11" t="n">
+      <c r="N11" t="n">
         <v>-75170</v>
       </c>
-      <c r="M11" t="n">
+      <c r="O11" t="n">
         <v>-6468</v>
       </c>
-      <c r="N11" t="n">
+      <c r="P11" t="n">
         <v>-59554</v>
       </c>
-      <c r="O11" t="n">
+      <c r="Q11" t="n">
         <v>48191</v>
       </c>
-      <c r="P11" t="n">
+      <c r="R11" t="n">
         <v>23619</v>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="n">
+        <v>0.01112191055688502</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.01251455145432362</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.02317539643266151</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.01153968234667085</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.009004260663373167</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.008747333439710899</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.01286518314108307</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.01203404136783002</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1061,33 +1293,57 @@
       <c r="I12" t="n">
         <v>462461</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="n">
         <v>336329</v>
       </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
         <v>-76296</v>
       </c>
-      <c r="L12" t="n">
+      <c r="N12" t="n">
         <v>-103730</v>
       </c>
-      <c r="M12" t="n">
+      <c r="O12" t="n">
         <v>-28191</v>
       </c>
-      <c r="N12" t="n">
+      <c r="P12" t="n">
         <v>51307</v>
       </c>
-      <c r="O12" t="n">
+      <c r="Q12" t="n">
         <v>198161</v>
       </c>
-      <c r="P12" t="n">
+      <c r="R12" t="n">
         <v>-36170</v>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="n">
+        <v>0.02806323346926811</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.01599166513901268</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.03492295973429068</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.01713657475736398</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.01374960778786946</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.01087908339542902</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.01208264328353259</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.01293404729701762</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1119,33 +1375,57 @@
       <c r="I13" t="n">
         <v>168128</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="n">
         <v>417</v>
       </c>
-      <c r="K13" t="n">
+      <c r="M13" t="n">
         <v>9087</v>
       </c>
-      <c r="L13" t="n">
+      <c r="N13" t="n">
         <v>-49509</v>
       </c>
-      <c r="M13" t="n">
+      <c r="O13" t="n">
         <v>-33223</v>
       </c>
-      <c r="N13" t="n">
+      <c r="P13" t="n">
         <v>-2518</v>
       </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
         <v>45197</v>
       </c>
-      <c r="P13" t="n">
+      <c r="R13" t="n">
         <v>-15626</v>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="n">
+        <v>0.004257393924246121</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.004156980580001464</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.007220995772934684</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.004285890245585258</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.003971330308059751</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.003444274192720851</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.004322463448736397</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.004702181381679705</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1177,33 +1457,57 @@
       <c r="I14" t="n">
         <v>1703777</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="n">
         <v>-63186</v>
       </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
         <v>272956</v>
       </c>
-      <c r="L14" t="n">
+      <c r="N14" t="n">
         <v>-1279011</v>
       </c>
-      <c r="M14" t="n">
+      <c r="O14" t="n">
         <v>-309418</v>
       </c>
-      <c r="N14" t="n">
+      <c r="P14" t="n">
         <v>-87905</v>
       </c>
-      <c r="O14" t="n">
+      <c r="Q14" t="n">
         <v>512026</v>
       </c>
-      <c r="P14" t="n">
+      <c r="R14" t="n">
         <v>224282</v>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="n">
+        <v>0.03398573541057627</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.03545921262960421</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.04904483581512185</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.05405755646434405</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.0478595955754504</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.04251069450804131</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.05464823120029409</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.0476510068991132</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1235,36 +1539,60 @@
       <c r="I15" t="n">
         <v>3535449</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Subtotals</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
         <v>466529</v>
       </c>
-      <c r="K15" t="n">
+      <c r="M15" t="n">
         <v>259314</v>
       </c>
-      <c r="L15" t="n">
+      <c r="N15" t="n">
         <v>-1892720</v>
       </c>
-      <c r="M15" t="n">
+      <c r="O15" t="n">
         <v>-646566</v>
       </c>
-      <c r="N15" t="n">
+      <c r="P15" t="n">
         <v>-83692</v>
       </c>
-      <c r="O15" t="n">
+      <c r="Q15" t="n">
         <v>1149825</v>
       </c>
-      <c r="P15" t="n">
+      <c r="R15" t="n">
         <v>174022</v>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>Subtotals</t>
-        </is>
+      <c r="S15" t="n">
+        <v>0.1034093974239159</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.08535984201249189</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.1436068157559227</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.1092666227531265</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.09716878643152448</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.08465772617763197</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.10513995102784</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0.09887896402549327</v>
       </c>
     </row>
     <row r="16">
@@ -1297,33 +1625,57 @@
       <c r="I16" t="n">
         <v>638306</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="n">
         <v>645068</v>
       </c>
-      <c r="K16" t="n">
+      <c r="M16" t="n">
         <v>-35710</v>
       </c>
-      <c r="L16" t="n">
+      <c r="N16" t="n">
         <v>-690035</v>
       </c>
-      <c r="M16" t="n">
+      <c r="O16" t="n">
         <v>-327382</v>
       </c>
-      <c r="N16" t="n">
+      <c r="P16" t="n">
         <v>-84520</v>
       </c>
-      <c r="O16" t="n">
+      <c r="Q16" t="n">
         <v>834268</v>
       </c>
-      <c r="P16" t="n">
+      <c r="R16" t="n">
         <v>-123154</v>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="n">
+        <v>0.0299124225516795</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.007243419631785233</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.01589230403892604</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.02480951389409971</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.02573680689547025</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.02350933733170816</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.01460128844568237</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.0178520567009329</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1355,33 +1707,57 @@
       <c r="I17" t="n">
         <v>1644017</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="n">
         <v>239093</v>
       </c>
-      <c r="K17" t="n">
+      <c r="M17" t="n">
         <v>310209</v>
       </c>
-      <c r="L17" t="n">
+      <c r="N17" t="n">
         <v>-902885</v>
       </c>
-      <c r="M17" t="n">
+      <c r="O17" t="n">
         <v>-1075956</v>
       </c>
-      <c r="N17" t="n">
+      <c r="P17" t="n">
         <v>84591</v>
       </c>
-      <c r="O17" t="n">
+      <c r="Q17" t="n">
         <v>376104</v>
       </c>
-      <c r="P17" t="n">
+      <c r="R17" t="n">
         <v>526071</v>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="n">
+        <v>0.0419355727791617</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.03290912175840071</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.0418649381159333</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.0411453455394151</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.05352830583831601</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.04435927038230993</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.06150821668267611</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.04597964722452491</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1413,33 +1789,57 @@
       <c r="I18" t="n">
         <v>1116001</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="n">
         <v>254775</v>
       </c>
-      <c r="K18" t="n">
+      <c r="M18" t="n">
         <v>116001</v>
       </c>
-      <c r="L18" t="n">
+      <c r="N18" t="n">
         <v>-553903</v>
       </c>
-      <c r="M18" t="n">
+      <c r="O18" t="n">
         <v>-435515</v>
       </c>
-      <c r="N18" t="n">
+      <c r="P18" t="n">
         <v>113714</v>
       </c>
-      <c r="O18" t="n">
+      <c r="Q18" t="n">
         <v>235682</v>
       </c>
-      <c r="P18" t="n">
+      <c r="R18" t="n">
         <v>-59347</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="n">
+        <v>0.0274885081556238</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.01821801801332872</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.02675433228280663</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.02568324188677984</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.0286087732906759</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0.02251483079390434</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0.02994943209243885</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.03121216646921353</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1471,33 +1871,57 @@
       <c r="I19" t="n">
         <v>396814</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="n">
         <v>161954</v>
       </c>
-      <c r="K19" t="n">
+      <c r="M19" t="n">
         <v>273897</v>
       </c>
-      <c r="L19" t="n">
+      <c r="N19" t="n">
         <v>-579849</v>
       </c>
-      <c r="M19" t="n">
+      <c r="O19" t="n">
         <v>-60336</v>
       </c>
-      <c r="N19" t="n">
+      <c r="P19" t="n">
         <v>260239</v>
       </c>
-      <c r="O19" t="n">
+      <c r="Q19" t="n">
         <v>176428</v>
       </c>
-      <c r="P19" t="n">
+      <c r="R19" t="n">
         <v>12682</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="n">
+        <v>0.02240632772465592</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.01641349934034527</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.0132270297407495</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.02079531899639121</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.01721680269830958</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0.01020785594310428</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.01160661166675689</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0.01109804079504812</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1529,33 +1953,57 @@
       <c r="I20" t="n">
         <v>408318</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="n">
         <v>-440665.4</v>
       </c>
-      <c r="K20" t="n">
+      <c r="M20" t="n">
         <v>112753</v>
       </c>
-      <c r="L20" t="n">
+      <c r="N20" t="n">
         <v>-72659.80000000005</v>
       </c>
-      <c r="M20" t="n">
+      <c r="O20" t="n">
         <v>-851045.2</v>
       </c>
-      <c r="N20" t="n">
+      <c r="P20" t="n">
         <v>175003</v>
       </c>
-      <c r="O20" t="n">
+      <c r="Q20" t="n">
         <v>607867</v>
       </c>
-      <c r="P20" t="n">
+      <c r="R20" t="n">
         <v>259648</v>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="n">
+        <v>0.00695474533006009</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.02188639877446729</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.03385010736229609</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.01587224798473542</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.02952003001738989</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.02222731868204504</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.0189325951134979</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.01141978312597958</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1587,33 +2035,57 @@
       <c r="I21" t="n">
         <v>480005</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="n">
         <v>532043</v>
       </c>
-      <c r="K21" t="n">
+      <c r="M21" t="n">
         <v>-437237</v>
       </c>
-      <c r="L21" t="n">
+      <c r="N21" t="n">
         <v>-608894</v>
       </c>
-      <c r="M21" t="n">
+      <c r="O21" t="n">
         <v>435333</v>
       </c>
-      <c r="N21" t="n">
+      <c r="P21" t="n">
         <v>113840</v>
       </c>
-      <c r="O21" t="n">
+      <c r="Q21" t="n">
         <v>2798</v>
       </c>
-      <c r="P21" t="n">
+      <c r="R21" t="n">
         <v>52236</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="n">
+        <v>0.01990309753484453</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.001302511004698491</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.03052289721384599</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0.02869147331373865</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0.01320268283779417</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0.00932134719851477</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0.0150856530958211</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.0134247155388345</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1645,36 +2117,60 @@
       <c r="I22" t="n">
         <v>16048330</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Subtotals</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
         <v>3133631.6</v>
       </c>
-      <c r="K22" t="n">
+      <c r="M22" t="n">
         <v>1627126</v>
       </c>
-      <c r="L22" t="n">
+      <c r="N22" t="n">
         <v>-8883088.800000001</v>
       </c>
-      <c r="M22" t="n">
+      <c r="O22" t="n">
         <v>-6577714.199999999</v>
       </c>
-      <c r="N22" t="n">
+      <c r="P22" t="n">
         <v>-748698</v>
       </c>
-      <c r="O22" t="n">
+      <c r="Q22" t="n">
         <v>8037904</v>
       </c>
-      <c r="P22" t="n">
+      <c r="R22" t="n">
         <v>298511</v>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>Subtotals</t>
-        </is>
+      <c r="S22" t="n">
+        <v>0.4515973745285323</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0.3352772983148117</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0.5249793450071556</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0.4514142070997856</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0.4809205292206964</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0.4248263668484859</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0.4633291545344031</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0.4488375436158871</v>
       </c>
     </row>
     <row r="23">
@@ -1691,23 +2187,31 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Account group</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>Account group</t>
-        </is>
-      </c>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1739,33 +2243,57 @@
       <c r="I24" t="n">
         <v>4811631</v>
       </c>
-      <c r="J24" t="n">
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="n">
         <v>23716</v>
       </c>
-      <c r="K24" t="n">
+      <c r="M24" t="n">
         <v>-291071</v>
       </c>
-      <c r="L24" t="n">
+      <c r="N24" t="n">
         <v>-65733</v>
       </c>
-      <c r="M24" t="n">
+      <c r="O24" t="n">
         <v>-156583</v>
       </c>
-      <c r="N24" t="n">
+      <c r="P24" t="n">
         <v>-143833</v>
       </c>
-      <c r="O24" t="n">
+      <c r="Q24" t="n">
         <v>-30317</v>
       </c>
-      <c r="P24" t="n">
+      <c r="R24" t="n">
         <v>46550</v>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="n">
+        <v>0.1464256129828783</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.1426514457782025</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.2865123314128118</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0.119809735984604</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0.09530555881049602</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0.08411012388108215</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.137698586247037</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0.1345710512449616</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1797,33 +2325,57 @@
       <c r="I25" t="n">
         <v>486360</v>
       </c>
-      <c r="J25" t="n">
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="n">
         <v>323300</v>
       </c>
-      <c r="K25" t="n">
+      <c r="M25" t="n">
         <v>-100</v>
       </c>
-      <c r="L25" t="n">
+      <c r="N25" t="n">
         <v>-352140</v>
       </c>
-      <c r="M25" t="n">
+      <c r="O25" t="n">
         <v>-1116420</v>
       </c>
-      <c r="N25" t="n">
+      <c r="P25" t="n">
         <v>742870</v>
       </c>
-      <c r="O25" t="n">
+      <c r="Q25" t="n">
         <v>249150</v>
       </c>
-      <c r="P25" t="n">
+      <c r="R25" t="n">
         <v>314080</v>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="n">
+        <v>0.02259033896976429</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.01107515725220901</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0.02079947825995379</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0.01789002853595042</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.03647102291711171</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0.01828575637680453</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0.02268739192211618</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0.01360245132752273</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1855,33 +2407,57 @@
       <c r="I26" t="n">
         <v>814738</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="n">
         <v>107431</v>
       </c>
-      <c r="K26" t="n">
+      <c r="M26" t="n">
         <v>88568</v>
       </c>
-      <c r="L26" t="n">
+      <c r="N26" t="n">
         <v>-516177</v>
       </c>
-      <c r="M26" t="n">
+      <c r="O26" t="n">
         <v>-277247</v>
       </c>
-      <c r="N26" t="n">
+      <c r="P26" t="n">
         <v>149659</v>
       </c>
-      <c r="O26" t="n">
+      <c r="Q26" t="n">
         <v>347916</v>
       </c>
-      <c r="P26" t="n">
+      <c r="R26" t="n">
         <v>-93750</v>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="n">
+        <v>0.02168400242157542</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.01757067883434383</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0.02730061558492898</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0.02491002026706512</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.02479399211081107</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0.01862224119341063</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0.0204354321712342</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0.02278648324221403</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1913,36 +2489,60 @@
       <c r="I27" t="n">
         <v>6112729</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Subtotals</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
         <v>454447</v>
       </c>
-      <c r="K27" t="n">
+      <c r="M27" t="n">
         <v>-202603</v>
       </c>
-      <c r="L27" t="n">
+      <c r="N27" t="n">
         <v>-934050</v>
       </c>
-      <c r="M27" t="n">
+      <c r="O27" t="n">
         <v>-1550250</v>
       </c>
-      <c r="N27" t="n">
+      <c r="P27" t="n">
         <v>748696</v>
       </c>
-      <c r="O27" t="n">
+      <c r="Q27" t="n">
         <v>566749</v>
       </c>
-      <c r="P27" t="n">
+      <c r="R27" t="n">
         <v>266880</v>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>Subtotals</t>
-        </is>
+      <c r="S27" t="n">
+        <v>0.190699954374218</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.1712972818647554</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0.3346124252576946</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0.1626097847876195</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.1565705738384188</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0.1210181214512973</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0.1808214103403874</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0.1709599858146983</v>
       </c>
     </row>
     <row r="28">
@@ -1959,23 +2559,31 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Account group</t>
+        </is>
+      </c>
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>Account group</t>
-        </is>
-      </c>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2007,33 +2615,57 @@
       <c r="I29" t="n">
         <v>1508278</v>
       </c>
-      <c r="J29" t="n">
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="n">
         <v>-129990</v>
       </c>
-      <c r="K29" t="n">
+      <c r="M29" t="n">
         <v>49474</v>
       </c>
-      <c r="L29" t="n">
+      <c r="N29" t="n">
         <v>-87841</v>
       </c>
-      <c r="M29" t="n">
+      <c r="O29" t="n">
         <v>-15410</v>
       </c>
-      <c r="N29" t="n">
+      <c r="P29" t="n">
         <v>-3760</v>
       </c>
-      <c r="O29" t="n">
+      <c r="Q29" t="n">
         <v>-11330</v>
       </c>
-      <c r="P29" t="n">
+      <c r="R29" t="n">
         <v>10880</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="n">
+        <v>0.04609186699446571</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.0496053146586271</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0.08995450057941863</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0.03939431705264611</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0.03060313674887829</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0.02626909123193287</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0.04305848400581952</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0.0421833170560353</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2065,33 +2697,57 @@
       <c r="I30" t="n">
         <v>2851817</v>
       </c>
-      <c r="J30" t="n">
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="n">
         <v>18697</v>
       </c>
-      <c r="K30" t="n">
+      <c r="M30" t="n">
         <v>-38931</v>
       </c>
-      <c r="L30" t="n">
+      <c r="N30" t="n">
         <v>-787812</v>
       </c>
-      <c r="M30" t="n">
+      <c r="O30" t="n">
         <v>-514604</v>
       </c>
-      <c r="N30" t="n">
+      <c r="P30" t="n">
         <v>-101793.79</v>
       </c>
-      <c r="O30" t="n">
+      <c r="Q30" t="n">
         <v>88209.79000000004</v>
       </c>
-      <c r="P30" t="n">
+      <c r="R30" t="n">
         <v>-521640</v>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="n">
+        <v>0.03469866989124468</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.03335701917723232</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.06512612677753984</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0.04768598697039932</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0.04713551007700065</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0.04213267244049804</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0.06604572341075024</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0.07975923582840259</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2123,33 +2779,57 @@
       <c r="I31" t="n">
         <v>1225202</v>
       </c>
-      <c r="J31" t="n">
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="n">
         <v>528798</v>
       </c>
-      <c r="K31" t="n">
+      <c r="M31" t="n">
         <v>-26190</v>
       </c>
-      <c r="L31" t="n">
+      <c r="N31" t="n">
         <v>-651592</v>
       </c>
-      <c r="M31" t="n">
+      <c r="O31" t="n">
         <v>-842665</v>
       </c>
-      <c r="N31" t="n">
+      <c r="P31" t="n">
         <v>424304</v>
       </c>
-      <c r="O31" t="n">
+      <c r="Q31" t="n">
         <v>455885</v>
       </c>
-      <c r="P31" t="n">
+      <c r="R31" t="n">
         <v>173727</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="n">
+        <v>0.04494569791850327</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.02594935339002674</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.05040043009134176</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.03801281752640611</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.04637300961181941</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0.03231421500613221</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.03965075520240626</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0.0342662854087168</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2181,33 +2861,57 @@
       <c r="I32" t="n">
         <v>119429</v>
       </c>
-      <c r="J32" t="n">
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="n">
         <v>76144</v>
       </c>
-      <c r="K32" t="n">
+      <c r="M32" t="n">
         <v>-11085</v>
       </c>
-      <c r="L32" t="n">
+      <c r="N32" t="n">
         <v>-39712</v>
       </c>
-      <c r="M32" t="n">
+      <c r="O32" t="n">
         <v>26334</v>
       </c>
-      <c r="N32" t="n">
+      <c r="P32" t="n">
         <v>-183628</v>
       </c>
-      <c r="O32" t="n">
+      <c r="Q32" t="n">
         <v>80669</v>
       </c>
-      <c r="P32" t="n">
+      <c r="R32" t="n">
         <v>161930</v>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="n">
+        <v>0.00803215543270335</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.005265214582869975</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.01059700988395831</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.005417870395655986</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.003629888805559248</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0.006307182623292704</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0.00797474127206872</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0.003340174273366873</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2239,33 +2943,57 @@
       <c r="I33" t="n">
         <v>115085</v>
       </c>
-      <c r="J33" t="n">
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="n">
         <v>-28794</v>
       </c>
-      <c r="K33" t="n">
+      <c r="M33" t="n">
         <v>6053</v>
       </c>
-      <c r="L33" t="n">
+      <c r="N33" t="n">
         <v>1447</v>
       </c>
-      <c r="M33" t="n">
+      <c r="O33" t="n">
         <v>-122158</v>
       </c>
-      <c r="N33" t="n">
+      <c r="P33" t="n">
         <v>16395</v>
       </c>
-      <c r="O33" t="n">
+      <c r="Q33" t="n">
         <v>79143</v>
       </c>
-      <c r="P33" t="n">
+      <c r="R33" t="n">
         <v>-22603</v>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="n">
+        <v>0.001555874250045518</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.002509251656382203</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.004322297259028187</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.001742904353935812</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.003825626083078754</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0.002990017948121721</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0.002621277522039315</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0.003218681863286358</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2297,33 +3025,57 @@
       <c r="I34" t="n">
         <v>429480</v>
       </c>
-      <c r="J34" t="n">
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="n">
         <v>-466582</v>
       </c>
-      <c r="K34" t="n">
+      <c r="M34" t="n">
         <v>394740</v>
       </c>
-      <c r="L34" t="n">
+      <c r="N34" t="n">
         <v>-37200</v>
       </c>
-      <c r="M34" t="n">
+      <c r="O34" t="n">
         <v>-91215</v>
       </c>
-      <c r="N34" t="n">
+      <c r="P34" t="n">
         <v>69930</v>
       </c>
-      <c r="O34" t="n">
+      <c r="Q34" t="n">
         <v>-423400</v>
       </c>
-      <c r="P34" t="n">
+      <c r="R34" t="n">
         <v>153635</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="n">
+        <v>0.001025938620991242</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.01696400785169272</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.006500559383313129</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0.00366326940747828</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.004672566226192004</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0.002782524204423951</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0.01652760799143568</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0.01201163910713147</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2355,33 +3107,57 @@
       <c r="I35" t="n">
         <v>231100</v>
       </c>
-      <c r="J35" t="n">
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="n">
         <v>62700</v>
       </c>
-      <c r="K35" t="n">
+      <c r="M35" t="n">
         <v>14600</v>
       </c>
-      <c r="L35" t="n">
+      <c r="N35" t="n">
         <v>-219800</v>
       </c>
-      <c r="M35" t="n">
+      <c r="O35" t="n">
         <v>-57100</v>
       </c>
-      <c r="N35" t="n">
+      <c r="P35" t="n">
         <v>6950</v>
       </c>
-      <c r="O35" t="n">
+      <c r="Q35" t="n">
         <v>98194</v>
       </c>
-      <c r="P35" t="n">
+      <c r="R35" t="n">
         <v>33356</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="n">
+        <v>0.005934720483480034</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.003670056742316327</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.005952799119165534</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0.008269679186859514</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0.007520218063535303</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0.006318018988412773</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0.007495648540996398</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0.006463373841990507</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2405,23 +3181,39 @@
       </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
-      <c r="M36" t="n">
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="n">
         <v>-781800</v>
       </c>
-      <c r="N36" t="n">
+      <c r="P36" t="n">
         <v>799100</v>
       </c>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
+      <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="n">
+        <v>0.0002736295800422238</v>
+      </c>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="n">
+        <v>0.0009764837183843714</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0.01665801549950312</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0.0003414674539442723</v>
+      </c>
+      <c r="Y36" t="inlineStr"/>
+      <c r="Z36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2453,36 +3245,60 @@
       <c r="I37" t="n">
         <v>6480391</v>
       </c>
-      <c r="J37" t="n">
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Cost of Sales</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Subtotals</t>
+        </is>
+      </c>
+      <c r="L37" t="n">
         <v>52973</v>
       </c>
-      <c r="K37" t="n">
+      <c r="M37" t="n">
         <v>396661</v>
       </c>
-      <c r="L37" t="n">
+      <c r="N37" t="n">
         <v>-1859410</v>
       </c>
-      <c r="M37" t="n">
+      <c r="O37" t="n">
         <v>-2398618</v>
       </c>
-      <c r="N37" t="n">
+      <c r="P37" t="n">
         <v>1027497.21</v>
       </c>
-      <c r="O37" t="n">
+      <c r="Q37" t="n">
         <v>386970.79</v>
       </c>
-      <c r="P37" t="n">
+      <c r="R37" t="n">
         <v>-10715</v>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>Cost of Sales</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>Subtotals</t>
-        </is>
+      <c r="S37" t="n">
+        <v>0.1422849235914338</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0.1375938476391896</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0.2328537230937654</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0.1451633286117655</v>
+      </c>
+      <c r="W37" t="n">
+        <v>0.1604179711155668</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0.1194551898967585</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0.1833742379455161</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>0.1812427073789299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple periods working well
</commit_message>
<xml_diff>
--- a/uploaded_files/cleaned_PL 8 Months.xlsx
+++ b/uploaded_files/cleaned_PL 8 Months.xlsx
@@ -481,17 +481,17 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>outliers</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Account type</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Account hierarchy</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>outliers</t>
         </is>
       </c>
     </row>
@@ -509,14 +509,14 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L2" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -549,15 +549,15 @@
       <c r="I3" t="n">
         <v>21502500</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -573,14 +573,14 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L4" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -613,15 +613,15 @@
       <c r="I5" t="n">
         <v>1141000</v>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -653,14 +653,14 @@
       <c r="I6" t="n">
         <v>1141000</v>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L6" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -677,14 +677,14 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L7" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -717,15 +717,15 @@
       <c r="I8" t="n">
         <v>9445710</v>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="b">
-        <v>0</v>
-      </c>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -757,15 +757,15 @@
       <c r="I9" t="n">
         <v>230310</v>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="b">
-        <v>0</v>
-      </c>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -797,14 +797,14 @@
       <c r="I10" t="n">
         <v>9676020</v>
       </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr">
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L10" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -837,15 +837,15 @@
       <c r="I11" t="n">
         <v>700840</v>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="b">
-        <v>0</v>
-      </c>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -877,15 +877,15 @@
       <c r="I12" t="n">
         <v>2318160</v>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -913,15 +913,15 @@
       <c r="I13" t="n">
         <v>232000</v>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -953,15 +953,15 @@
       <c r="I14" t="n">
         <v>184800</v>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>Income</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="b">
-        <v>0</v>
-      </c>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -993,18 +993,18 @@
       <c r="I15" t="n">
         <v>35755320</v>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>Key KPI</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L15" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1021,14 +1021,14 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr">
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L16" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1045,14 +1045,14 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr">
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L17" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1069,14 +1069,14 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr">
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L18" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1109,15 +1109,15 @@
       <c r="I19" t="n">
         <v>2559356</v>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="b">
-        <v>0</v>
-      </c>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1149,15 +1149,15 @@
       <c r="I20" t="n">
         <v>4113591</v>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="b">
-        <v>0</v>
-      </c>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1189,15 +1189,15 @@
       <c r="I21" t="n">
         <v>673301</v>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="b">
-        <v>0</v>
-      </c>
+      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1229,15 +1229,15 @@
       <c r="I22" t="n">
         <v>483172</v>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="b">
-        <v>0</v>
-      </c>
+      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1269,14 +1269,14 @@
       <c r="I23" t="n">
         <v>7829420</v>
       </c>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr">
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L23" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1293,14 +1293,14 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr">
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L24" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1333,15 +1333,15 @@
       <c r="I25" t="n">
         <v>770802</v>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="b">
-        <v>0</v>
-      </c>
+      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1373,15 +1373,15 @@
       <c r="I26" t="n">
         <v>430281</v>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="b">
-        <v>0</v>
-      </c>
+      <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1413,15 +1413,15 @@
       <c r="I27" t="n">
         <v>462461</v>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="b">
-        <v>0</v>
-      </c>
+      <c r="L27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1453,15 +1453,15 @@
       <c r="I28" t="n">
         <v>168128</v>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="b">
-        <v>0</v>
-      </c>
+      <c r="L28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1493,15 +1493,15 @@
       <c r="I29" t="n">
         <v>1703777</v>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="b">
-        <v>0</v>
-      </c>
+      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1533,14 +1533,14 @@
       <c r="I30" t="n">
         <v>3535449</v>
       </c>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr">
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L30" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1573,15 +1573,15 @@
       <c r="I31" t="n">
         <v>638306</v>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="b">
-        <v>0</v>
-      </c>
+      <c r="L31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1613,15 +1613,15 @@
       <c r="I32" t="n">
         <v>1644017</v>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="b">
-        <v>0</v>
-      </c>
+      <c r="L32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1653,15 +1653,15 @@
       <c r="I33" t="n">
         <v>1116001</v>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="b">
-        <v>0</v>
-      </c>
+      <c r="L33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1693,15 +1693,15 @@
       <c r="I34" t="n">
         <v>396814</v>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="b">
-        <v>0</v>
-      </c>
+      <c r="L34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1733,15 +1733,15 @@
       <c r="I35" t="n">
         <v>408318</v>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="b">
-        <v>0</v>
-      </c>
+      <c r="L35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1773,15 +1773,15 @@
       <c r="I36" t="n">
         <v>480005</v>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="b">
-        <v>0</v>
-      </c>
+      <c r="L36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1813,14 +1813,14 @@
       <c r="I37" t="n">
         <v>16048330</v>
       </c>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr">
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L37" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1837,14 +1837,14 @@
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr">
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L38" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1877,15 +1877,15 @@
       <c r="I39" t="n">
         <v>4811631</v>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="b">
-        <v>0</v>
-      </c>
+      <c r="L39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1917,15 +1917,15 @@
       <c r="I40" t="n">
         <v>486360</v>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="b">
-        <v>0</v>
-      </c>
+      <c r="L40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1957,15 +1957,15 @@
       <c r="I41" t="n">
         <v>814738</v>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="J41" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="b">
-        <v>0</v>
-      </c>
+      <c r="L41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1997,14 +1997,14 @@
       <c r="I42" t="n">
         <v>6112729</v>
       </c>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr">
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L42" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -2021,14 +2021,14 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr">
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L43" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2061,15 +2061,15 @@
       <c r="I44" t="n">
         <v>1508278</v>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="b">
-        <v>0</v>
-      </c>
+      <c r="L44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2101,15 +2101,15 @@
       <c r="I45" t="n">
         <v>2851817</v>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="b">
-        <v>0</v>
-      </c>
+      <c r="L45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2141,15 +2141,15 @@
       <c r="I46" t="n">
         <v>1225202</v>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="J46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="b">
-        <v>0</v>
-      </c>
+      <c r="L46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2181,15 +2181,15 @@
       <c r="I47" t="n">
         <v>119429</v>
       </c>
-      <c r="J47" t="inlineStr">
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="b">
-        <v>0</v>
-      </c>
+      <c r="L47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2221,15 +2221,15 @@
       <c r="I48" t="n">
         <v>115085</v>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="J48" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="b">
-        <v>0</v>
-      </c>
+      <c r="L48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2261,15 +2261,15 @@
       <c r="I49" t="n">
         <v>429480</v>
       </c>
-      <c r="J49" t="inlineStr">
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr"/>
-      <c r="L49" t="b">
-        <v>0</v>
-      </c>
+      <c r="L49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2301,15 +2301,15 @@
       <c r="I50" t="n">
         <v>231100</v>
       </c>
-      <c r="J50" t="inlineStr">
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="b">
-        <v>0</v>
-      </c>
+      <c r="L50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2333,15 +2333,15 @@
       </c>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr">
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="inlineStr">
         <is>
           <t>Cost of Sales</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="b">
-        <v>0</v>
-      </c>
+      <c r="L51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2373,14 +2373,14 @@
       <c r="I52" t="n">
         <v>6480391</v>
       </c>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr">
+      <c r="J52" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L52" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2413,18 +2413,18 @@
       <c r="I53" t="n">
         <v>28641450</v>
       </c>
-      <c r="J53" t="inlineStr">
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr">
         <is>
           <t>Key KPI</t>
         </is>
       </c>
-      <c r="K53" t="inlineStr">
+      <c r="L53" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L53" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2457,15 +2457,15 @@
       <c r="I54" t="n">
         <v>7113870</v>
       </c>
-      <c r="J54" t="inlineStr">
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="inlineStr">
         <is>
           <t>Key KPI</t>
         </is>
       </c>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="b">
-        <v>0</v>
-      </c>
+      <c r="L54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2481,14 +2481,14 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr">
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L55" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2505,14 +2505,14 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr">
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L56" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2545,15 +2545,15 @@
       <c r="I57" t="n">
         <v>6438800</v>
       </c>
-      <c r="J57" t="inlineStr">
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" t="inlineStr">
         <is>
           <t>Other Income(Loss)</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="b">
-        <v>0</v>
-      </c>
+      <c r="L57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2585,15 +2585,15 @@
       <c r="I58" t="n">
         <v>872291</v>
       </c>
-      <c r="J58" t="inlineStr">
+      <c r="J58" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" t="inlineStr">
         <is>
           <t>Other Income(Loss)</t>
         </is>
       </c>
-      <c r="K58" t="inlineStr"/>
-      <c r="L58" t="b">
-        <v>0</v>
-      </c>
+      <c r="L58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2625,14 +2625,14 @@
       <c r="I59" t="n">
         <v>7311091</v>
       </c>
-      <c r="J59" t="inlineStr"/>
-      <c r="K59" t="inlineStr">
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L59" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2665,14 +2665,14 @@
       <c r="I60" t="n">
         <v>7311091</v>
       </c>
-      <c r="J60" t="inlineStr"/>
-      <c r="K60" t="inlineStr">
+      <c r="J60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L60" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2689,14 +2689,14 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
-      <c r="K61" t="inlineStr">
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L61" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2713,14 +2713,14 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr"/>
-      <c r="J62" t="inlineStr"/>
-      <c r="K62" t="inlineStr">
+      <c r="J62" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L62" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2737,14 +2737,14 @@
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
-      <c r="J63" t="inlineStr"/>
-      <c r="K63" t="inlineStr">
+      <c r="J63" t="b">
+        <v>0</v>
+      </c>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L63" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2777,15 +2777,15 @@
       <c r="I64" t="n">
         <v>629600</v>
       </c>
-      <c r="J64" t="inlineStr">
+      <c r="J64" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K64" t="inlineStr"/>
-      <c r="L64" t="b">
-        <v>0</v>
-      </c>
+      <c r="L64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2817,15 +2817,15 @@
       <c r="I65" t="n">
         <v>0</v>
       </c>
-      <c r="J65" t="inlineStr">
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K65" t="inlineStr"/>
-      <c r="L65" t="b">
-        <v>0</v>
-      </c>
+      <c r="L65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2857,15 +2857,15 @@
       <c r="I66" t="n">
         <v>1254148</v>
       </c>
-      <c r="J66" t="inlineStr">
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K66" t="inlineStr"/>
-      <c r="L66" t="b">
-        <v>0</v>
-      </c>
+      <c r="L66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2897,15 +2897,15 @@
       <c r="I67" t="n">
         <v>510500</v>
       </c>
-      <c r="J67" t="inlineStr">
+      <c r="J67" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K67" t="inlineStr"/>
-      <c r="L67" t="b">
-        <v>0</v>
-      </c>
+      <c r="L67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2937,14 +2937,14 @@
       <c r="I68" t="n">
         <v>2394248</v>
       </c>
-      <c r="J68" t="inlineStr"/>
-      <c r="K68" t="inlineStr">
+      <c r="J68" t="b">
+        <v>0</v>
+      </c>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L68" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2977,15 +2977,15 @@
       <c r="I69" t="n">
         <v>208569.25</v>
       </c>
-      <c r="J69" t="inlineStr">
+      <c r="J69" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K69" t="inlineStr"/>
-      <c r="L69" t="b">
-        <v>0</v>
-      </c>
+      <c r="L69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3001,14 +3001,14 @@
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
-      <c r="K70" t="inlineStr">
+      <c r="J70" t="b">
+        <v>0</v>
+      </c>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L70" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -3041,15 +3041,15 @@
       <c r="I71" t="n">
         <v>262285</v>
       </c>
-      <c r="J71" t="inlineStr">
+      <c r="J71" t="b">
+        <v>0</v>
+      </c>
+      <c r="K71" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K71" t="inlineStr"/>
-      <c r="L71" t="b">
-        <v>0</v>
-      </c>
+      <c r="L71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3081,14 +3081,14 @@
       <c r="I72" t="n">
         <v>262285</v>
       </c>
-      <c r="J72" t="inlineStr"/>
-      <c r="K72" t="inlineStr">
+      <c r="J72" t="b">
+        <v>0</v>
+      </c>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L72" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -3121,14 +3121,14 @@
       <c r="I73" t="n">
         <v>2865102.25</v>
       </c>
-      <c r="J73" t="inlineStr"/>
-      <c r="K73" t="inlineStr">
+      <c r="J73" t="b">
+        <v>0</v>
+      </c>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L73" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -3145,14 +3145,14 @@
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
-      <c r="J74" t="inlineStr"/>
-      <c r="K74" t="inlineStr">
+      <c r="J74" t="b">
+        <v>0</v>
+      </c>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L74" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -3185,15 +3185,15 @@
       <c r="I75" t="n">
         <v>323800</v>
       </c>
-      <c r="J75" t="inlineStr">
+      <c r="J75" t="b">
+        <v>0</v>
+      </c>
+      <c r="K75" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K75" t="inlineStr"/>
-      <c r="L75" t="b">
-        <v>0</v>
-      </c>
+      <c r="L75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3225,15 +3225,15 @@
       <c r="I76" t="n">
         <v>60</v>
       </c>
-      <c r="J76" t="inlineStr">
+      <c r="J76" t="b">
+        <v>0</v>
+      </c>
+      <c r="K76" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K76" t="inlineStr"/>
-      <c r="L76" t="b">
-        <v>0</v>
-      </c>
+      <c r="L76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3265,14 +3265,14 @@
       <c r="I77" t="n">
         <v>323860</v>
       </c>
-      <c r="J77" t="inlineStr"/>
-      <c r="K77" t="inlineStr">
+      <c r="J77" t="b">
+        <v>0</v>
+      </c>
+      <c r="K77" t="inlineStr"/>
+      <c r="L77" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L77" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -3289,14 +3289,14 @@
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr"/>
-      <c r="J78" t="inlineStr"/>
-      <c r="K78" t="inlineStr">
+      <c r="J78" t="b">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr"/>
+      <c r="L78" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L78" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -3329,15 +3329,15 @@
       <c r="I79" t="n">
         <v>224127</v>
       </c>
-      <c r="J79" t="inlineStr">
+      <c r="J79" t="b">
+        <v>0</v>
+      </c>
+      <c r="K79" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K79" t="inlineStr"/>
-      <c r="L79" t="b">
-        <v>0</v>
-      </c>
+      <c r="L79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3355,14 +3355,14 @@
       <c r="I80" t="n">
         <v>129290</v>
       </c>
-      <c r="J80" t="inlineStr"/>
-      <c r="K80" t="inlineStr">
+      <c r="J80" t="b">
+        <v>0</v>
+      </c>
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L80" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -3395,15 +3395,15 @@
       <c r="I81" t="n">
         <v>5600</v>
       </c>
-      <c r="J81" t="inlineStr">
+      <c r="J81" t="b">
+        <v>0</v>
+      </c>
+      <c r="K81" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K81" t="inlineStr"/>
-      <c r="L81" t="b">
-        <v>0</v>
-      </c>
+      <c r="L81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3435,14 +3435,14 @@
       <c r="I82" t="n">
         <v>359017</v>
       </c>
-      <c r="J82" t="inlineStr"/>
-      <c r="K82" t="inlineStr">
+      <c r="J82" t="b">
+        <v>0</v>
+      </c>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L82" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -3459,14 +3459,14 @@
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="inlineStr"/>
-      <c r="J83" t="inlineStr"/>
-      <c r="K83" t="inlineStr">
+      <c r="J83" t="b">
+        <v>0</v>
+      </c>
+      <c r="K83" t="inlineStr"/>
+      <c r="L83" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L83" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -3485,14 +3485,14 @@
       <c r="I84" t="n">
         <v>32000</v>
       </c>
-      <c r="J84" t="inlineStr"/>
-      <c r="K84" t="inlineStr">
+      <c r="J84" t="b">
+        <v>0</v>
+      </c>
+      <c r="K84" t="inlineStr"/>
+      <c r="L84" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L84" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -3525,15 +3525,15 @@
       <c r="I85" t="n">
         <v>32000</v>
       </c>
-      <c r="J85" t="inlineStr">
+      <c r="J85" t="b">
+        <v>0</v>
+      </c>
+      <c r="K85" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K85" t="inlineStr"/>
-      <c r="L85" t="b">
-        <v>0</v>
-      </c>
+      <c r="L85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3565,15 +3565,15 @@
       <c r="I86" t="n">
         <v>484012.5</v>
       </c>
-      <c r="J86" t="inlineStr">
+      <c r="J86" t="b">
+        <v>0</v>
+      </c>
+      <c r="K86" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K86" t="inlineStr"/>
-      <c r="L86" t="b">
-        <v>0</v>
-      </c>
+      <c r="L86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3591,14 +3591,14 @@
         <v>30770</v>
       </c>
       <c r="I87" t="inlineStr"/>
-      <c r="J87" t="inlineStr"/>
-      <c r="K87" t="inlineStr">
+      <c r="J87" t="b">
+        <v>0</v>
+      </c>
+      <c r="K87" t="inlineStr"/>
+      <c r="L87" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L87" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -3631,15 +3631,15 @@
       <c r="I88" t="n">
         <v>51959</v>
       </c>
-      <c r="J88" t="inlineStr">
+      <c r="J88" t="b">
+        <v>0</v>
+      </c>
+      <c r="K88" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K88" t="inlineStr"/>
-      <c r="L88" t="b">
-        <v>0</v>
-      </c>
+      <c r="L88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3671,14 +3671,14 @@
       <c r="I89" t="n">
         <v>599971.5</v>
       </c>
-      <c r="J89" t="inlineStr"/>
-      <c r="K89" t="inlineStr">
+      <c r="J89" t="b">
+        <v>0</v>
+      </c>
+      <c r="K89" t="inlineStr"/>
+      <c r="L89" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L89" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -3695,14 +3695,14 @@
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="inlineStr"/>
-      <c r="J90" t="inlineStr"/>
-      <c r="K90" t="inlineStr">
+      <c r="J90" t="b">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L90" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -3735,15 +3735,15 @@
       <c r="I91" t="n">
         <v>27608</v>
       </c>
-      <c r="J91" t="inlineStr">
+      <c r="J91" t="b">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K91" t="inlineStr"/>
-      <c r="L91" t="b">
-        <v>0</v>
-      </c>
+      <c r="L91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3775,15 +3775,15 @@
       <c r="I92" t="n">
         <v>88468</v>
       </c>
-      <c r="J92" t="inlineStr">
+      <c r="J92" t="b">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K92" t="inlineStr"/>
-      <c r="L92" t="b">
-        <v>0</v>
-      </c>
+      <c r="L92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3815,15 +3815,15 @@
       <c r="I93" t="n">
         <v>3190</v>
       </c>
-      <c r="J93" t="inlineStr">
+      <c r="J93" t="b">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="b">
-        <v>0</v>
-      </c>
+      <c r="L93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3855,15 +3855,15 @@
       <c r="I94" t="n">
         <v>6430</v>
       </c>
-      <c r="J94" t="inlineStr">
+      <c r="J94" t="b">
+        <v>0</v>
+      </c>
+      <c r="K94" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="b">
-        <v>0</v>
-      </c>
+      <c r="L94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3895,14 +3895,14 @@
       <c r="I95" t="n">
         <v>125696</v>
       </c>
-      <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr">
+      <c r="J95" t="b">
+        <v>0</v>
+      </c>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L95" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3919,14 +3919,14 @@
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr"/>
-      <c r="J96" t="inlineStr"/>
-      <c r="K96" t="inlineStr">
+      <c r="J96" t="b">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr"/>
+      <c r="L96" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L96" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -3959,15 +3959,15 @@
       <c r="I97" t="n">
         <v>23000</v>
       </c>
-      <c r="J97" t="inlineStr">
+      <c r="J97" t="b">
+        <v>0</v>
+      </c>
+      <c r="K97" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="b">
-        <v>0</v>
-      </c>
+      <c r="L97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3999,15 +3999,15 @@
       <c r="I98" t="n">
         <v>18450</v>
       </c>
-      <c r="J98" t="inlineStr">
+      <c r="J98" t="b">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="b">
-        <v>0</v>
-      </c>
+      <c r="L98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4039,15 +4039,15 @@
       <c r="I99" t="n">
         <v>65182</v>
       </c>
-      <c r="J99" t="inlineStr">
+      <c r="J99" t="b">
+        <v>0</v>
+      </c>
+      <c r="K99" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K99" t="inlineStr"/>
-      <c r="L99" t="b">
-        <v>0</v>
-      </c>
+      <c r="L99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4079,14 +4079,14 @@
       <c r="I100" t="n">
         <v>106632</v>
       </c>
-      <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr">
+      <c r="J100" t="b">
+        <v>0</v>
+      </c>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L100" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -4103,14 +4103,14 @@
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
       <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr">
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L101" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -4143,15 +4143,15 @@
       <c r="I102" t="n">
         <v>423349</v>
       </c>
-      <c r="J102" t="inlineStr">
+      <c r="J102" t="b">
+        <v>0</v>
+      </c>
+      <c r="K102" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K102" t="inlineStr"/>
-      <c r="L102" t="b">
-        <v>0</v>
-      </c>
+      <c r="L102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4173,15 +4173,15 @@
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
       <c r="I103" t="inlineStr"/>
-      <c r="J103" t="inlineStr">
+      <c r="J103" t="b">
+        <v>0</v>
+      </c>
+      <c r="K103" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K103" t="inlineStr"/>
-      <c r="L103" t="b">
-        <v>0</v>
-      </c>
+      <c r="L103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4213,14 +4213,14 @@
       <c r="I104" t="n">
         <v>423349</v>
       </c>
-      <c r="J104" t="inlineStr"/>
-      <c r="K104" t="inlineStr">
+      <c r="J104" t="b">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L104" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -4237,14 +4237,14 @@
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr"/>
-      <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr">
+      <c r="J105" t="b">
+        <v>0</v>
+      </c>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L105" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -4277,15 +4277,15 @@
       <c r="I106" t="n">
         <v>34833</v>
       </c>
-      <c r="J106" t="inlineStr">
+      <c r="J106" t="b">
+        <v>0</v>
+      </c>
+      <c r="K106" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K106" t="inlineStr"/>
-      <c r="L106" t="b">
-        <v>0</v>
-      </c>
+      <c r="L106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4317,15 +4317,15 @@
       <c r="I107" t="n">
         <v>24178</v>
       </c>
-      <c r="J107" t="inlineStr">
+      <c r="J107" t="b">
+        <v>0</v>
+      </c>
+      <c r="K107" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K107" t="inlineStr"/>
-      <c r="L107" t="b">
-        <v>0</v>
-      </c>
+      <c r="L107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4357,14 +4357,14 @@
       <c r="I108" t="n">
         <v>59011</v>
       </c>
-      <c r="J108" t="inlineStr"/>
-      <c r="K108" t="inlineStr">
+      <c r="J108" t="b">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L108" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -4381,14 +4381,14 @@
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="inlineStr"/>
       <c r="I109" t="inlineStr"/>
-      <c r="J109" t="inlineStr"/>
-      <c r="K109" t="inlineStr">
+      <c r="J109" t="b">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L109" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -4421,15 +4421,15 @@
       <c r="I110" t="n">
         <v>140000</v>
       </c>
-      <c r="J110" t="inlineStr">
+      <c r="J110" t="b">
+        <v>0</v>
+      </c>
+      <c r="K110" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K110" t="inlineStr"/>
-      <c r="L110" t="b">
-        <v>0</v>
-      </c>
+      <c r="L110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4461,15 +4461,15 @@
       <c r="I111" t="n">
         <v>333895</v>
       </c>
-      <c r="J111" t="inlineStr">
+      <c r="J111" t="b">
+        <v>0</v>
+      </c>
+      <c r="K111" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K111" t="inlineStr"/>
-      <c r="L111" t="b">
-        <v>0</v>
-      </c>
+      <c r="L111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4491,15 +4491,15 @@
         <v>15000</v>
       </c>
       <c r="I112" t="inlineStr"/>
-      <c r="J112" t="inlineStr">
+      <c r="J112" t="b">
+        <v>0</v>
+      </c>
+      <c r="K112" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K112" t="inlineStr"/>
-      <c r="L112" t="b">
-        <v>0</v>
-      </c>
+      <c r="L112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4531,14 +4531,14 @@
       <c r="I113" t="n">
         <v>473895</v>
       </c>
-      <c r="J113" t="inlineStr"/>
-      <c r="K113" t="inlineStr">
+      <c r="J113" t="b">
+        <v>0</v>
+      </c>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L113" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -4555,14 +4555,14 @@
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
-      <c r="J114" t="inlineStr"/>
-      <c r="K114" t="inlineStr">
+      <c r="J114" t="b">
+        <v>0</v>
+      </c>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L114" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -4595,15 +4595,15 @@
       <c r="I115" t="n">
         <v>10000</v>
       </c>
-      <c r="J115" t="inlineStr">
+      <c r="J115" t="b">
+        <v>0</v>
+      </c>
+      <c r="K115" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K115" t="inlineStr"/>
-      <c r="L115" t="b">
-        <v>0</v>
-      </c>
+      <c r="L115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4635,15 +4635,15 @@
       <c r="I116" t="n">
         <v>20490</v>
       </c>
-      <c r="J116" t="inlineStr">
+      <c r="J116" t="b">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K116" t="inlineStr"/>
-      <c r="L116" t="b">
-        <v>0</v>
-      </c>
+      <c r="L116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4675,14 +4675,14 @@
       <c r="I117" t="n">
         <v>30490</v>
       </c>
-      <c r="J117" t="inlineStr"/>
-      <c r="K117" t="inlineStr">
+      <c r="J117" t="b">
+        <v>0</v>
+      </c>
+      <c r="K117" t="inlineStr"/>
+      <c r="L117" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L117" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -4715,18 +4715,18 @@
       <c r="I118" t="n">
         <v>5367023.75</v>
       </c>
-      <c r="J118" t="inlineStr">
+      <c r="J118" t="b">
+        <v>0</v>
+      </c>
+      <c r="K118" t="inlineStr">
         <is>
           <t>Key KPI</t>
         </is>
       </c>
-      <c r="K118" t="inlineStr">
+      <c r="L118" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L118" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -4743,14 +4743,14 @@
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
       <c r="I119" t="inlineStr"/>
-      <c r="J119" t="inlineStr"/>
-      <c r="K119" t="inlineStr">
+      <c r="J119" t="b">
+        <v>0</v>
+      </c>
+      <c r="K119" t="inlineStr"/>
+      <c r="L119" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L119" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -4767,14 +4767,14 @@
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
       <c r="I120" t="inlineStr"/>
-      <c r="J120" t="inlineStr"/>
-      <c r="K120" t="inlineStr">
+      <c r="J120" t="b">
+        <v>0</v>
+      </c>
+      <c r="K120" t="inlineStr"/>
+      <c r="L120" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L120" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -4807,15 +4807,15 @@
       <c r="I121" t="n">
         <v>3103700</v>
       </c>
-      <c r="J121" t="inlineStr">
+      <c r="J121" t="b">
+        <v>0</v>
+      </c>
+      <c r="K121" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K121" t="inlineStr"/>
-      <c r="L121" t="b">
-        <v>0</v>
-      </c>
+      <c r="L121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4847,15 +4847,15 @@
       <c r="I122" t="n">
         <v>24491.4</v>
       </c>
-      <c r="J122" t="inlineStr">
+      <c r="J122" t="b">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K122" t="inlineStr"/>
-      <c r="L122" t="b">
-        <v>0</v>
-      </c>
+      <c r="L122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4883,15 +4883,15 @@
       <c r="I123" t="n">
         <v>119362</v>
       </c>
-      <c r="J123" t="inlineStr">
+      <c r="J123" t="b">
+        <v>0</v>
+      </c>
+      <c r="K123" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K123" t="inlineStr"/>
-      <c r="L123" t="b">
-        <v>0</v>
-      </c>
+      <c r="L123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -4923,15 +4923,15 @@
       <c r="I124" t="n">
         <v>771180</v>
       </c>
-      <c r="J124" t="inlineStr">
+      <c r="J124" t="b">
+        <v>0</v>
+      </c>
+      <c r="K124" t="inlineStr">
         <is>
           <t>Expenses</t>
         </is>
       </c>
-      <c r="K124" t="inlineStr"/>
-      <c r="L124" t="b">
-        <v>0</v>
-      </c>
+      <c r="L124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4963,14 +4963,14 @@
       <c r="I125" t="n">
         <v>4018733.4</v>
       </c>
-      <c r="J125" t="inlineStr"/>
-      <c r="K125" t="inlineStr">
+      <c r="J125" t="b">
+        <v>0</v>
+      </c>
+      <c r="K125" t="inlineStr"/>
+      <c r="L125" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L125" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -5003,14 +5003,14 @@
       <c r="I126" t="n">
         <v>4018733.4</v>
       </c>
-      <c r="J126" t="inlineStr"/>
-      <c r="K126" t="inlineStr">
+      <c r="J126" t="b">
+        <v>0</v>
+      </c>
+      <c r="K126" t="inlineStr"/>
+      <c r="L126" t="inlineStr">
         <is>
           <t>Subtotals</t>
         </is>
-      </c>
-      <c r="L126" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -5043,15 +5043,15 @@
       <c r="I127" t="n">
         <v>5039203.85</v>
       </c>
-      <c r="J127" t="inlineStr">
+      <c r="J127" t="b">
+        <v>0</v>
+      </c>
+      <c r="K127" t="inlineStr">
         <is>
           <t>Key KPI</t>
         </is>
       </c>
-      <c r="K127" t="inlineStr"/>
-      <c r="L127" t="b">
-        <v>0</v>
-      </c>
+      <c r="L127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5067,14 +5067,14 @@
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr"/>
       <c r="I128" t="inlineStr"/>
-      <c r="J128" t="inlineStr"/>
-      <c r="K128" t="inlineStr">
+      <c r="J128" t="b">
+        <v>0</v>
+      </c>
+      <c r="K128" t="inlineStr"/>
+      <c r="L128" t="inlineStr">
         <is>
           <t>Account group</t>
         </is>
-      </c>
-      <c r="L128" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>